<commit_message>
Previsão de Vendas no jupyter
</commit_message>
<xml_diff>
--- a/Tabela com Previsao.xlsx
+++ b/Tabela com Previsao.xlsx
@@ -466,7 +466,7 @@
         <v>69.2</v>
       </c>
       <c r="D2" t="n">
-        <v>7.568999999999997</v>
+        <v>7.743999999999997</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>5.1</v>
       </c>
       <c r="D3" t="n">
-        <v>8.458000000000002</v>
+        <v>8.572000000000003</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>20.07600000000001</v>
+        <v>19.71200000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>